<commit_message>
últimas correcciones sobre la carga de excel
</commit_message>
<xml_diff>
--- a/client/src/assets/muestras-ejemplo.xlsx
+++ b/client/src/assets/muestras-ejemplo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Carga de Muestras</t>
   </si>
@@ -30,12 +30,15 @@
   <si>
     <t>Notas</t>
   </si>
+  <si>
+    <t>Escriba desde aquí...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -51,6 +54,16 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -79,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -87,7 +100,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -335,43 +354,49 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4">
-      <c r="C4" s="3"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5">
-      <c r="C5" s="3"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6">
-      <c r="C6" s="3"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7">
-      <c r="C7" s="3"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8">
-      <c r="C8" s="3"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9">
-      <c r="C9" s="3"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10">
-      <c r="C10" s="3"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11">
-      <c r="C11" s="3"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12">
-      <c r="C12" s="3"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13">
-      <c r="C13" s="3"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14">
-      <c r="C14" s="3"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15">
-      <c r="C15" s="3"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>